<commit_message>
Added Role command to switch between roles
</commit_message>
<xml_diff>
--- a/data/attributes.xlsx
+++ b/data/attributes.xlsx
@@ -188,7 +188,7 @@
   <dimension ref="A2:L13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="L17" activeCellId="0" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -247,7 +247,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>-0.5</v>
+        <v>-0.7</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>0.7</v>
@@ -264,7 +264,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>-0.5</v>
+        <v>-0.7</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0.5</v>
@@ -366,11 +366,17 @@
       <c r="C9" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="D9" s="0" t="n">
+        <v>1.5</v>
+      </c>
       <c r="F9" s="0" t="n">
         <v>0.7</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>0.7</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="L9" s="0" t="n">
         <v>0.5</v>

</xml_diff>